<commit_message>
-fix file carga producto
</commit_message>
<xml_diff>
--- a/src/templates/plantilla_carga_producto.xlsx
+++ b/src/templates/plantilla_carga_producto.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APRENDIZAJE\PROYECTOS\KathyGirl\komercia-backend\src\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APRENDIZAJE\PROYECTOS\KathyGirl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F075F42E-DBEF-45E2-92FB-F3F0FB426315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695DFC08-2067-4C59-A939-2E7313DE7E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FFFEFAB0-B4F3-49F9-B75A-75560AC37488}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Nombre</t>
   </si>
@@ -101,6 +101,18 @@
   </si>
   <si>
     <t>Id Categoria</t>
+  </si>
+  <si>
+    <t>Pantalones</t>
+  </si>
+  <si>
+    <t>Polos</t>
+  </si>
+  <si>
+    <t>Tops m/l</t>
+  </si>
+  <si>
+    <t>Polos m/l</t>
   </si>
 </sst>
 </file>
@@ -499,7 +511,7 @@
   <dimension ref="A1:F1411"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,12 +541,6 @@
       </c>
       <c r="F1" s="3" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E2" t="str">
-        <f>IFERROR( VLOOKUP(Hoja1!F2,CATEGORIAS,2,FALSE),"")</f>
-        <v/>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9011,10 +9017,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9061BE1-22B5-477D-94A7-F45AD9F1A862}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9035,7 +9041,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -9043,7 +9049,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -9051,7 +9057,7 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -9059,7 +9065,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -9067,7 +9073,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -9075,7 +9081,7 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -9083,7 +9089,7 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -9091,7 +9097,7 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -9099,7 +9105,7 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -9107,7 +9113,7 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -9115,7 +9121,7 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -9123,7 +9129,7 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -9131,6 +9137,38 @@
         <v>18</v>
       </c>
       <c r="B14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
-fix file plantilla carga producto
</commit_message>
<xml_diff>
--- a/src/templates/plantilla_carga_producto.xlsx
+++ b/src/templates/plantilla_carga_producto.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APRENDIZAJE\PROYECTOS\KathyGirl\komercia-backend\src\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APRENDIZAJE\PROYECTOS\KathyGirl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F075F42E-DBEF-45E2-92FB-F3F0FB426315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695DFC08-2067-4C59-A939-2E7313DE7E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FFFEFAB0-B4F3-49F9-B75A-75560AC37488}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Nombre</t>
   </si>
@@ -101,6 +101,18 @@
   </si>
   <si>
     <t>Id Categoria</t>
+  </si>
+  <si>
+    <t>Pantalones</t>
+  </si>
+  <si>
+    <t>Polos</t>
+  </si>
+  <si>
+    <t>Tops m/l</t>
+  </si>
+  <si>
+    <t>Polos m/l</t>
   </si>
 </sst>
 </file>
@@ -499,7 +511,7 @@
   <dimension ref="A1:F1411"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,12 +541,6 @@
       </c>
       <c r="F1" s="3" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E2" t="str">
-        <f>IFERROR( VLOOKUP(Hoja1!F2,CATEGORIAS,2,FALSE),"")</f>
-        <v/>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9011,10 +9017,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9061BE1-22B5-477D-94A7-F45AD9F1A862}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9035,7 +9041,7 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -9043,7 +9049,7 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -9051,7 +9057,7 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -9059,7 +9065,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -9067,7 +9073,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -9075,7 +9081,7 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -9083,7 +9089,7 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -9091,7 +9097,7 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -9099,7 +9105,7 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -9107,7 +9113,7 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -9115,7 +9121,7 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -9123,7 +9129,7 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -9131,6 +9137,38 @@
         <v>18</v>
       </c>
       <c r="B14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix template carga producto
</commit_message>
<xml_diff>
--- a/src/templates/plantilla_carga_producto.xlsx
+++ b/src/templates/plantilla_carga_producto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APRENDIZAJE\PROYECTOS\KathyGirl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695DFC08-2067-4C59-A939-2E7313DE7E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611A1904-AEAE-4606-B982-A9A540094495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FFFEFAB0-B4F3-49F9-B75A-75560AC37488}"/>
   </bookViews>
@@ -17,7 +17,8 @@
     <sheet name="categoria_producto" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="CATEGORIAS">categoria_producto!$A$2:$B$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">categoria_producto!$A$1:$B$18</definedName>
+    <definedName name="CATEGORIAS">categoria_producto!$A$2:$B$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -508,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7C7AC8-E151-4842-A811-76D66930074E}">
-  <dimension ref="A1:F1411"/>
+  <dimension ref="A1:F1410"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,6 +544,12 @@
         <v>19</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" t="str">
+        <f>IFERROR( VLOOKUP(Hoja1!F2,CATEGORIAS,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E3" t="str">
         <f>IFERROR( VLOOKUP(Hoja1!F3,CATEGORIAS,2,FALSE),"")</f>
@@ -8988,12 +8995,6 @@
     <row r="1410" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E1410" t="str">
         <f>IFERROR( VLOOKUP(Hoja1!F1410,CATEGORIAS,2,FALSE),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1411" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E1411" t="str">
-        <f>IFERROR( VLOOKUP(Hoja1!F1411,CATEGORIAS,2,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -9003,11 +9004,11 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{809281BD-891F-43D8-AA5F-890617BBDE93}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4E84EAE8-63EB-4448-B029-5B1627A97C45}">
           <x14:formula1>
-            <xm:f>categoria_producto!$A$2:$A$14</xm:f>
+            <xm:f>categoria_producto!$A$2:$A$18</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>F2:F1500</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -9020,7 +9021,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9046,133 +9047,138 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
         <v>7</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B14">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B17">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B18" xr:uid="{F9061BE1-22B5-477D-94A7-F45AD9F1A862}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B18">
+      <sortCondition ref="A1:A18"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>